<commit_message>
Add function comments, switch log statements to debug, correct the plebdex btc ticker
</commit_message>
<xml_diff>
--- a/data/plebdex-weights.xlsx
+++ b/data/plebdex-weights.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hunter/Projects/stock-plotter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hunter/Projects/interactive-plebdex/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F36C918E-D11A-774A-A620-FB8FD6EE9058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19586D1-1593-D346-8817-2BFD30BEC26C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="760" windowWidth="15140" windowHeight="17440" activeTab="2" xr2:uid="{024AFAA7-7B3C-B340-ACE6-17FCF4F0F49F}"/>
+    <workbookView xWindow="40" yWindow="760" windowWidth="15140" windowHeight="17440" xr2:uid="{024AFAA7-7B3C-B340-ACE6-17FCF4F0F49F}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="1" r:id="rId1"/>
@@ -61,9 +61,6 @@
     <t>URNM</t>
   </si>
   <si>
-    <t>BTCUSD</t>
-  </si>
-  <si>
     <t>TSLA</t>
   </si>
   <si>
@@ -116,6 +113,9 @@
   </si>
   <si>
     <t>KTOS</t>
+  </si>
+  <si>
+    <t>BTC-USD</t>
   </si>
 </sst>
 </file>
@@ -489,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99690001-6801-514D-BE5C-0B0632EDED62}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -545,7 +545,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B7">
         <v>0.05</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>0.05</v>
@@ -561,7 +561,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>0.05</v>
@@ -569,7 +569,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>0.05</v>
@@ -600,7 +600,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>0.15</v>
@@ -616,7 +616,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>0.1</v>
@@ -624,7 +624,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>0.1</v>
@@ -632,7 +632,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>0.1</v>
@@ -640,7 +640,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>2.5000000000000001E-2</v>
@@ -648,7 +648,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>2.5000000000000001E-2</v>
@@ -656,7 +656,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9">
         <v>0.05</v>
@@ -680,7 +680,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>0.05</v>
@@ -688,7 +688,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>0.05</v>
@@ -696,7 +696,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>0.05</v>
@@ -704,7 +704,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15">
         <v>0.05</v>
@@ -719,7 +719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA23A9D5-DC6C-F245-974B-E2DBAA10DD49}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -743,7 +743,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>0.15</v>
@@ -751,7 +751,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>0.1</v>
@@ -759,7 +759,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>7.4999999999999997E-2</v>
@@ -767,7 +767,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>7.4999999999999997E-2</v>
@@ -775,7 +775,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>7.4999999999999997E-2</v>
@@ -783,7 +783,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>0.05</v>
@@ -799,7 +799,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10">
         <v>0.05</v>
@@ -807,7 +807,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>0.05</v>
@@ -815,7 +815,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12">
         <v>0.05</v>
@@ -831,7 +831,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>2.5000000000000001E-2</v>
@@ -839,7 +839,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>2.5000000000000001E-2</v>
@@ -847,7 +847,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>2.5000000000000001E-2</v>

</xml_diff>

<commit_message>
MVP: Successfully Plots the Plebdex against other benchmarks
</commit_message>
<xml_diff>
--- a/data/plebdex-weights.xlsx
+++ b/data/plebdex-weights.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hunter/Projects/interactive-plebdex/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19586D1-1593-D346-8817-2BFD30BEC26C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FD830A-7176-EC4C-B097-CEE9D5DA3C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="760" windowWidth="15140" windowHeight="17440" xr2:uid="{024AFAA7-7B3C-B340-ACE6-17FCF4F0F49F}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="2024" sheetId="2" r:id="rId2"/>
     <sheet name="2025" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -490,7 +490,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>